<commit_message>
Incluye Enmascaramiento de PRESTAMOANEXO
</commit_message>
<xml_diff>
--- a/ENMASCARAR DATOS.xlsx
+++ b/ENMASCARAR DATOS.xlsx
@@ -15,7 +15,7 @@
     <sheet name="ENMASCARAR_COLUMNAS" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ENMASCARAR_COLUMNAS!$A$1:$F$380</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ENMASCARAR_COLUMNAS!$A$1:$F$391</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2280" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2346" uniqueCount="275">
   <si>
     <t>OWNER</t>
   </si>
@@ -816,6 +816,42 @@
   </si>
   <si>
     <t>NOMBREGRUPOECONOMICO</t>
+  </si>
+  <si>
+    <t>AGVIRTUAL</t>
+  </si>
+  <si>
+    <t>OPER_FRECUENTE</t>
+  </si>
+  <si>
+    <t>PAC_CLIENTE_MAE</t>
+  </si>
+  <si>
+    <t>PAC_CLIENTE_PACINET</t>
+  </si>
+  <si>
+    <t>PAC_USUARIO_MAE</t>
+  </si>
+  <si>
+    <t>NOMBRESOCIO_EMPRESA</t>
+  </si>
+  <si>
+    <t>DES_NOMBRE_CORTO</t>
+  </si>
+  <si>
+    <t>DES_NOMBRES</t>
+  </si>
+  <si>
+    <t>DES_APELLIDOS</t>
+  </si>
+  <si>
+    <t>DES_CELULAR</t>
+  </si>
+  <si>
+    <t>DES_EMAIL</t>
+  </si>
+  <si>
+    <t>APELLIDO</t>
   </si>
 </sst>
 </file>
@@ -1155,7 +1191,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F380"/>
+  <dimension ref="A1:F391"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5240,7 +5276,7 @@
         <v>16</v>
       </c>
       <c r="E204" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F204" t="s">
         <v>16</v>
@@ -5260,7 +5296,7 @@
         <v>13</v>
       </c>
       <c r="E205" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F205" t="s">
         <v>120</v>
@@ -5280,7 +5316,7 @@
         <v>13</v>
       </c>
       <c r="E206" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F206" s="2" t="s">
         <v>14</v>
@@ -8764,6 +8800,226 @@
       </c>
       <c r="F380" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>263</v>
+      </c>
+      <c r="B381" t="s">
+        <v>264</v>
+      </c>
+      <c r="C381" t="s">
+        <v>268</v>
+      </c>
+      <c r="D381" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E381" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F381" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>263</v>
+      </c>
+      <c r="B382" t="s">
+        <v>265</v>
+      </c>
+      <c r="C382" t="s">
+        <v>269</v>
+      </c>
+      <c r="D382" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E382" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F382" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>263</v>
+      </c>
+      <c r="B383" t="s">
+        <v>265</v>
+      </c>
+      <c r="C383" t="s">
+        <v>270</v>
+      </c>
+      <c r="D383" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E383" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F383" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>263</v>
+      </c>
+      <c r="B384" t="s">
+        <v>265</v>
+      </c>
+      <c r="C384" t="s">
+        <v>271</v>
+      </c>
+      <c r="D384" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E384" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F384" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>263</v>
+      </c>
+      <c r="B385" t="s">
+        <v>265</v>
+      </c>
+      <c r="C385" t="s">
+        <v>272</v>
+      </c>
+      <c r="D385" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E385" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F385" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>263</v>
+      </c>
+      <c r="B386" t="s">
+        <v>266</v>
+      </c>
+      <c r="C386" t="s">
+        <v>270</v>
+      </c>
+      <c r="D386" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E386" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F386" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>263</v>
+      </c>
+      <c r="B387" t="s">
+        <v>266</v>
+      </c>
+      <c r="C387" t="s">
+        <v>273</v>
+      </c>
+      <c r="D387" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E387" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F387" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>263</v>
+      </c>
+      <c r="B388" t="s">
+        <v>266</v>
+      </c>
+      <c r="C388" t="s">
+        <v>271</v>
+      </c>
+      <c r="D388" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E388" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F388" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>263</v>
+      </c>
+      <c r="B389" t="s">
+        <v>266</v>
+      </c>
+      <c r="C389" t="s">
+        <v>272</v>
+      </c>
+      <c r="D389" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E389" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F389" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>263</v>
+      </c>
+      <c r="B390" t="s">
+        <v>267</v>
+      </c>
+      <c r="C390" t="s">
+        <v>270</v>
+      </c>
+      <c r="D390" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E390" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F390" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>263</v>
+      </c>
+      <c r="B391" t="s">
+        <v>267</v>
+      </c>
+      <c r="C391" t="s">
+        <v>271</v>
+      </c>
+      <c r="D391" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E391" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F391" s="2" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>